<commit_message>
Frames in Ascii umwandeln funktioniert
</commit_message>
<xml_diff>
--- a/res/Mappe1.xlsx
+++ b/res/Mappe1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d-kas\Documents\ASCIINATOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d-kas\Documents\ASCIINATOR\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1640949E-2910-43E5-A1A6-343FB3EE8803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097A03E3-3789-434F-AEFB-3465C354627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8855E81-171A-4508-894B-CCE7ECC14887}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F8855E81-171A-4508-894B-CCE7ECC14887}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -105,6 +105,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75E27583-0643-4901-A465-69E892E344D1}" name="Tabelle1" displayName="Tabelle1" ref="D7:I71" totalsRowShown="0">
+  <autoFilter ref="D7:I71" xr:uid="{75E27583-0643-4901-A465-69E892E344D1}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1BC2A731-08C2-409B-A54A-1B926F1F549F}" name="Erstes x"/>
+    <tableColumn id="2" xr3:uid="{9F37CF7F-2BF8-4AD2-9FFA-B02B51566B8B}" name="Erstes y"/>
+    <tableColumn id="3" xr3:uid="{310E0BAD-EF56-42F5-9812-1F4767D9AE68}" name="Letzes x"/>
+    <tableColumn id="4" xr3:uid="{38C91276-5AE4-4072-AF92-E441BC7934BB}" name="Letzes y"/>
+    <tableColumn id="5" xr3:uid="{1EDA13DD-144A-4926-8410-E3D979490058}" name="Breite">
+      <calculatedColumnFormula>F8-D8+1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{BE30881F-F01B-4A6A-91D3-2C9A1B79699C}" name="Höhe">
+      <calculatedColumnFormula>G8-E8+1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60483332-2455-4B7E-BFFC-A6A13959220C}">
-  <dimension ref="C7:I39"/>
+  <dimension ref="C7:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,11 +490,11 @@
         <v>22</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H72" si="0">F9-D9+1</f>
+        <f t="shared" ref="H9:H39" si="0">F9-D9+1</f>
         <v>8</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I72" si="1">G9-E9+1</f>
+        <f t="shared" ref="I9:I39" si="1">G9-E9+1</f>
         <v>8</v>
       </c>
     </row>
@@ -1140,8 +1159,715 @@
         <v>15</v>
       </c>
     </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>59</v>
+      </c>
+      <c r="F40">
+        <v>21</v>
+      </c>
+      <c r="G40">
+        <v>74</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:H60" si="2">F40-D40+1</f>
+        <v>16</v>
+      </c>
+      <c r="I40">
+        <f t="shared" ref="I40:I60" si="3">G40-E40+1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>37</v>
+      </c>
+      <c r="E41">
+        <v>59</v>
+      </c>
+      <c r="F41">
+        <v>50</v>
+      </c>
+      <c r="G41">
+        <v>74</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>68</v>
+      </c>
+      <c r="E42">
+        <v>59</v>
+      </c>
+      <c r="F42">
+        <v>81</v>
+      </c>
+      <c r="G42">
+        <v>74</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>97</v>
+      </c>
+      <c r="E43">
+        <v>59</v>
+      </c>
+      <c r="F43">
+        <v>110</v>
+      </c>
+      <c r="G43">
+        <v>74</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>127</v>
+      </c>
+      <c r="E44">
+        <v>59</v>
+      </c>
+      <c r="F44">
+        <v>140</v>
+      </c>
+      <c r="G44">
+        <v>74</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>158</v>
+      </c>
+      <c r="E45">
+        <v>59</v>
+      </c>
+      <c r="F45">
+        <v>170</v>
+      </c>
+      <c r="G45">
+        <v>74</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>187</v>
+      </c>
+      <c r="E46">
+        <v>59</v>
+      </c>
+      <c r="F46">
+        <v>201</v>
+      </c>
+      <c r="G46">
+        <v>74</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>217</v>
+      </c>
+      <c r="E47">
+        <v>59</v>
+      </c>
+      <c r="F47">
+        <v>230</v>
+      </c>
+      <c r="G47">
+        <v>74</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>248</v>
+      </c>
+      <c r="E48">
+        <v>59</v>
+      </c>
+      <c r="F48">
+        <v>259</v>
+      </c>
+      <c r="G48">
+        <v>74</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>277</v>
+      </c>
+      <c r="E49">
+        <v>59</v>
+      </c>
+      <c r="F49">
+        <v>291</v>
+      </c>
+      <c r="G49">
+        <v>74</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>307</v>
+      </c>
+      <c r="E50">
+        <v>59</v>
+      </c>
+      <c r="F50">
+        <v>321</v>
+      </c>
+      <c r="G50">
+        <v>74</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>337</v>
+      </c>
+      <c r="E51">
+        <v>59</v>
+      </c>
+      <c r="F51">
+        <v>350</v>
+      </c>
+      <c r="G51">
+        <v>74</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>366</v>
+      </c>
+      <c r="E52">
+        <v>59</v>
+      </c>
+      <c r="F52">
+        <v>381</v>
+      </c>
+      <c r="G52">
+        <v>74</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>396</v>
+      </c>
+      <c r="E53">
+        <v>59</v>
+      </c>
+      <c r="F53">
+        <v>411</v>
+      </c>
+      <c r="G53">
+        <v>74</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>427</v>
+      </c>
+      <c r="E54">
+        <v>59</v>
+      </c>
+      <c r="F54">
+        <v>440</v>
+      </c>
+      <c r="G54">
+        <v>74</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>457</v>
+      </c>
+      <c r="E55">
+        <v>59</v>
+      </c>
+      <c r="F55">
+        <v>469</v>
+      </c>
+      <c r="G55">
+        <v>74</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>487</v>
+      </c>
+      <c r="E56">
+        <v>59</v>
+      </c>
+      <c r="F56">
+        <v>500</v>
+      </c>
+      <c r="G56">
+        <v>77</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>517</v>
+      </c>
+      <c r="E57">
+        <v>59</v>
+      </c>
+      <c r="F57">
+        <v>531</v>
+      </c>
+      <c r="G57">
+        <v>74</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>548</v>
+      </c>
+      <c r="E58">
+        <v>59</v>
+      </c>
+      <c r="F58">
+        <v>559</v>
+      </c>
+      <c r="G58">
+        <v>75</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>577</v>
+      </c>
+      <c r="E59">
+        <v>59</v>
+      </c>
+      <c r="F59">
+        <v>590</v>
+      </c>
+      <c r="G59">
+        <v>74</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>606</v>
+      </c>
+      <c r="E60">
+        <v>59</v>
+      </c>
+      <c r="F60">
+        <v>621</v>
+      </c>
+      <c r="G60">
+        <v>75</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>636</v>
+      </c>
+      <c r="E61">
+        <v>59</v>
+      </c>
+      <c r="F61">
+        <v>651</v>
+      </c>
+      <c r="G61">
+        <v>74</v>
+      </c>
+      <c r="H61">
+        <f t="shared" ref="H61:H90" si="4">F61-D61+1</f>
+        <v>16</v>
+      </c>
+      <c r="I61">
+        <f t="shared" ref="I61:I90" si="5">G61-E61+1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>666</v>
+      </c>
+      <c r="E62">
+        <v>59</v>
+      </c>
+      <c r="F62">
+        <v>681</v>
+      </c>
+      <c r="G62">
+        <v>74</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>696</v>
+      </c>
+      <c r="E63">
+        <v>59</v>
+      </c>
+      <c r="F63">
+        <v>710</v>
+      </c>
+      <c r="G63">
+        <v>74</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>726</v>
+      </c>
+      <c r="E64">
+        <v>59</v>
+      </c>
+      <c r="F64">
+        <v>740</v>
+      </c>
+      <c r="G64">
+        <v>74</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>758</v>
+      </c>
+      <c r="E65">
+        <v>59</v>
+      </c>
+      <c r="F65">
+        <v>769</v>
+      </c>
+      <c r="G65">
+        <v>74</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>794</v>
+      </c>
+      <c r="E66">
+        <v>57</v>
+      </c>
+      <c r="F66">
+        <v>798</v>
+      </c>
+      <c r="G66">
+        <v>76</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>818</v>
+      </c>
+      <c r="E67">
+        <v>56</v>
+      </c>
+      <c r="F67">
+        <v>829</v>
+      </c>
+      <c r="G67">
+        <v>78</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>849</v>
+      </c>
+      <c r="E68">
+        <v>57</v>
+      </c>
+      <c r="F68">
+        <v>853</v>
+      </c>
+      <c r="G68">
+        <v>77</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>877</v>
+      </c>
+      <c r="E69">
+        <v>59</v>
+      </c>
+      <c r="F69">
+        <v>889</v>
+      </c>
+      <c r="G69">
+        <v>70</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>904</v>
+      </c>
+      <c r="E70">
+        <v>76</v>
+      </c>
+      <c r="F70">
+        <v>922</v>
+      </c>
+      <c r="G70">
+        <v>77</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>941</v>
+      </c>
+      <c r="E71">
+        <v>58</v>
+      </c>
+      <c r="F71">
+        <v>945</v>
+      </c>
+      <c r="G71">
+        <v>61</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>